<commit_message>
Squashed bugs in electric and gas with no supplier case
</commit_message>
<xml_diff>
--- a/3.17.20 EG.xlsx
+++ b/3.17.20 EG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Electric Choice Id</t>
+          <t>Electric Choice ID</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Rate Code</t>
+          <t>Electric Rate Code</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -486,7 +486,22 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Usage (in kWh)</t>
+          <t>Electric Usage (kWh)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Choice ID</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Rate Code</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Gas Usage (therms)</t>
         </is>
       </c>
     </row>
@@ -505,6 +520,9 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>